<commit_message>
Correção na comparação entre heurísticas
</commit_message>
<xml_diff>
--- a/Comparaçoes/ComparaçãoEntreHeurísticas.xlsx
+++ b/Comparaçoes/ComparaçãoEntreHeurísticas.xlsx
@@ -99,9 +99,6 @@
     <t>2333.91</t>
   </si>
   <si>
-    <t>Comparação de rotas</t>
-  </si>
-  <si>
     <t xml:space="preserve">Problemas </t>
   </si>
   <si>
@@ -117,8 +114,56 @@
     <t>1 ,8 ,9 ,11 ,10 ,2 ,14</t>
   </si>
   <si>
-    <r>
-      <t>1</t>
+    <t>1,8,9,11,10,2,14,12,6,7</t>
+  </si>
+  <si>
+    <t>1,28,6,12,9,5,21</t>
+  </si>
+  <si>
+    <t>1,28,6,12,9,5,21,2,20,10,4,15,19,25</t>
+  </si>
+  <si>
+    <t>1,28,6,12,9,5,21,2,20,10,4,15,19,25,7,23,27,24,8,16,13</t>
+  </si>
+  <si>
+    <t>1,28,6,12,9,5,26</t>
+  </si>
+  <si>
+    <t>1,28,6,12,9,5,26,29,3,2,21,20,10,4</t>
+  </si>
+  <si>
+    <t>1,28,6,12,9,5,26,29,3,2,21,20,10,4,15,19,16,27,24,8,23</t>
+  </si>
+  <si>
+    <t>1,98,103,34,87,76,73,48,63,30,84,7,8,89,96,35,93,126,33,105,111,16,59,79,121,88,94,10,113,3,62,149,125,22,104,4,45</t>
+  </si>
+  <si>
+    <t>1,98,103,34,87,76,73,48,63,30,84,7,8,89,96,35,93,126,33,105,111,16,59,79,121,88,94,10,113,3,62,149,125,22,104,4,45,71,44,115,150,21,78,15,133,77,122,14,80,72,49,147,144,129,27,31,145,112,136,64,106,13,74,123,117,57,39,41,101,116,12,24,118,53,40</t>
+  </si>
+  <si>
+    <t>1,98,103,34,87,76,73,48,63,30,84,7,8,89,96,35,93,126,33,105,111,16,59,79,121,88,94,10,113,3,62,149,125,22,104,4,45,71,44,115,150,21,78,15,133,77,122,14,80,72,49,147,144,129,27,31,145,112,136,64,106,13,74,123,117,57,39,41,101,116,12,24,118,53,40,139,120,47,110,81,29,86,135,70,108,102,114,99,19,2,37,9,28,6,42,20,25,141,58,55,50,137,132,65,85,142,18,75,26,146,56,83</t>
+  </si>
+  <si>
+    <t>Legenda</t>
+  </si>
+  <si>
+    <t>Identificação</t>
+  </si>
+  <si>
+    <t>Significado</t>
+  </si>
+  <si>
+    <t>Números vermelhos</t>
+  </si>
+  <si>
+    <t>Células preenchidas</t>
+  </si>
+  <si>
+    <t>Indica qual dentre as 2 heurísticas apresentou um melhor resultado ,se não houver uma célula preenchida em uma coluna implica que os resultados são equivalentes</t>
+  </si>
+  <si>
+    <r>
+      <t>1,8,9,11,10,2</t>
     </r>
     <r>
       <rPr>
@@ -128,15 +173,12 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> ,2 ,8 ,13 ,9 ,11 ,10</t>
-    </r>
-  </si>
-  <si>
-    <t>1,8,9,11,10,2,14,12,6,7</t>
-  </si>
-  <si>
-    <r>
-      <t>1</t>
+      <t>,13</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>1,8,9,11,10,2,</t>
     </r>
     <r>
       <rPr>
@@ -146,21 +188,12 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>,2,8,12,6,7,13,9,11,10,</t>
-    </r>
-  </si>
-  <si>
-    <t>1,28,6,12,9,5,21</t>
-  </si>
-  <si>
-    <t>1,28,6,12,9,5,21,2,20,10,4,15,19,25</t>
-  </si>
-  <si>
-    <t>1,28,6,12,9,5,21,2,20,10,4,15,19,25,7,23,27,24,8,16,13</t>
-  </si>
-  <si>
-    <r>
-      <t>1,28,6,12,9</t>
+      <t>13,7,12,6,</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>1,28,6,12,9,5,21,2,20,10,4,15,19,25,</t>
     </r>
     <r>
       <rPr>
@@ -170,18 +203,15 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>,26,29,5,21,2,20,10,13,4,15,19,16,24,27,25,7</t>
-    </r>
-  </si>
-  <si>
-    <t>1,28,6,12,9,5,26</t>
-  </si>
-  <si>
-    <t>1,28,6,12,9,5,26,29,3,2,21,20,10,4</t>
-  </si>
-  <si>
-    <r>
-      <t>1</t>
+      <t>26,29,13,7,16,27,24</t>
+    </r>
+  </si>
+  <si>
+    <t>Comparação de ordem de inserção</t>
+  </si>
+  <si>
+    <r>
+      <t>1,28,6,12,9,5,26,29,3</t>
     </r>
     <r>
       <rPr>
@@ -191,15 +221,12 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>,24,13,16,27,8,28,6,12,9,5,26,29,3</t>
-    </r>
-  </si>
-  <si>
-    <t>1,28,6,12,9,5,26,29,3,2,21,20,10,4,15,19,16,27,24,8,23</t>
-  </si>
-  <si>
-    <r>
-      <t>1</t>
+      <t>,8,24,27,16,13</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>1,28,6,12,9,5,26,29,3,</t>
     </r>
     <r>
       <rPr>
@@ -209,15 +236,15 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>,24,13,21,2,20,10,4,15,19,16,27,8,28,6,12,9,5,26,29,3</t>
-    </r>
-  </si>
-  <si>
-    <t>1,98,103,34,87,76,73,48,63,30,84,7,8,89,96,35,93,126,33,105,111,16,59,79,121,88,94,10,113,3,62,149,125,22,104,4,45</t>
-  </si>
-  <si>
-    <r>
-      <t>1</t>
+      <t>8,24,27,16,13,19,4,10,15,20,2,21</t>
+    </r>
+  </si>
+  <si>
+    <t>Indicam a partir de qual ponto a ordem de inserção difere da rota do vizinho mais próximo</t>
+  </si>
+  <si>
+    <r>
+      <t>1,98,103</t>
     </r>
     <r>
       <rPr>
@@ -227,15 +254,12 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>,87,98,103,34,76,73,48,63,30,96,35,93,52,121,10,94,88,79,59,78,15,80,14,122,77,133,16,111,105,33,126,124,89,8,84,7</t>
-    </r>
-  </si>
-  <si>
-    <t>1,98,103,34,87,76,73,48,63,30,84,7,8,89,96,35,93,126,33,105,111,16,59,79,121,88,94,10,113,3,62,149,125,22,104,4,45,71,44,115,150,21,78,15,133,77,122,14,80,72,49,147,144,129,27,31,145,112,136,64,106,13,74,123,117,57,39,41,101,116,12,24,118,53,40</t>
-  </si>
-  <si>
-    <r>
-      <t>1</t>
+      <t>,87,34,30,84,7,8,89,96,63,48,73,76,35,93,124,126,52,33,105,111,16,59,79,121,15,78,133,88,94,122,77,14,80,10</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>1,98,103</t>
     </r>
     <r>
       <rPr>
@@ -245,21 +269,12 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>,87,98,103,34,76,73,48,63,30,96,35,93,52,121,10,113,3,62,149,22,125,150,115,4,104,68,119,91,13,106,128,45,71,44,21,94,88,79,59,78,15,80,14,122,77,133,16,111,105,54,134,138,46,90,109,43,51,20,25,81,141,83,75,26,146,56,92,33,126,124,89,8,84,7</t>
-    </r>
-  </si>
-  <si>
-    <t>1,98,103,34,87,76,73,48,63,30,84,7,8,89,96,35,93,126,33,105,111,16,59,79,121,88,94,10,113,3,62,149,125,22,104,4,45,71,44,115,150,21,78,15,133,77,122,14,80,72,49,147,144,129,27,31,145,112,136,64,106,13,74,123,117,57,39,41,101,116,12,24,118,53,40,139,120,47,110,81,29,86,135,70,108,102,114,99,19,2,37,9,28,6,42,20,25,141,58,55,50,137,132,65,85,142,18,75,26,146,56,83</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>1,</t>
+      <t>,87,34,30,84,7,8,89,96,63,48,73,76,35,93,124,126,52,33,105,111,16,59,79,121,15,78,133,88,94,122,77,14,80,10,113,3,62,149,125,22,21,150,115,44,71,45,4,128,104,68,119,91,106,13,92,54,46,138,134,90,56,83,26,146,75,141,25,20,51,109,43,81</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>1,98,103</t>
     </r>
     <r>
       <rPr>
@@ -269,36 +284,15 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>87,98,103,34,76,73,48,63,30,96,35,93,52,121,10,113,3,62,149,22,125,150,115,4,104,68,119,91,13,106,128,45,71,44,64,21,94,88,79,59,78,15,80,14,122,77,133,16,111,105,54,134,138,46,90,109,131,32,23,38,67,43,51,20,25,47,139,53,12,24,127,69,61,36,118,40,120,42,28,9,6,37,99,114,102,19,2,110,81,29,86,108,70,135,50,58,55,141,83,75,26,146,56,92,33,126,124,89,8,84,7</t>
-    </r>
-  </si>
-  <si>
-    <t>Legenda</t>
-  </si>
-  <si>
-    <t>Identificação</t>
-  </si>
-  <si>
-    <t>Significado</t>
-  </si>
-  <si>
-    <t>Números vermelhos</t>
-  </si>
-  <si>
-    <t>Indicam a partir de qual ponto aquela rota difere da rota do vizinho mais próximo</t>
-  </si>
-  <si>
-    <t>Células preenchidas</t>
-  </si>
-  <si>
-    <t>Indica qual dentre as 2 heurísticas apresentou um melhor resultado ,se não houver uma célula preenchida em uma coluna implica que os resultados são equivalentes</t>
+      <t>,87,34,30,84,7,8,89,96,63,48,73,76,35,93,124,126,52,33,105,111,16,59,79,121,15,78,133,88,94,122,77,14,80,10,113,3,62,149,125,22,21,150,115,44,71,45,4,128,104,68,119,91,106,13,92,54,46,138,134,90,56,83,26,146,75,141,25,20,51,109,43,81,110,58,55,86,29,135,50,70,108,67,47,120,42,37,2,9,28,6,139,40,53,118,24,12,19,99,114,102,32,131,38,23,127,69,36,61,64</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -317,12 +311,6 @@
       <u/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -412,7 +400,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -427,63 +415,70 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -788,8 +783,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B9:O34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D5" workbookViewId="0">
-      <selection activeCell="E29" sqref="E29"/>
+    <sheetView tabSelected="1" topLeftCell="F17" workbookViewId="0">
+      <selection activeCell="K29" sqref="K29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -807,16 +802,16 @@
     <row r="9" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B9" s="3"/>
       <c r="C9" s="1"/>
-      <c r="D9" s="6" t="s">
+      <c r="D9" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="E9" s="6"/>
-      <c r="G9" s="10"/>
-      <c r="H9" s="10"/>
-      <c r="I9" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="J9" s="6"/>
+      <c r="E9" s="16"/>
+      <c r="G9" s="6"/>
+      <c r="H9" s="6"/>
+      <c r="I9" s="16" t="s">
+        <v>51</v>
+      </c>
+      <c r="J9" s="16"/>
     </row>
     <row r="10" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B10" s="3" t="s">
@@ -832,25 +827,25 @@
         <v>2</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H10" s="2" t="s">
         <v>4</v>
       </c>
       <c r="I10" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="J10" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="J10" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="K10" s="12"/>
-      <c r="L10" s="12"/>
-      <c r="M10" s="12"/>
-      <c r="N10" s="12"/>
-      <c r="O10" s="12"/>
+      <c r="K10" s="7"/>
+      <c r="L10" s="7"/>
+      <c r="M10" s="7"/>
+      <c r="N10" s="7"/>
+      <c r="O10" s="7"/>
     </row>
     <row r="11" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B11" s="7" t="s">
+      <c r="B11" s="24" t="s">
         <v>5</v>
       </c>
       <c r="C11" s="1">
@@ -862,21 +857,21 @@
       <c r="E11" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="G11" s="5" t="s">
+      <c r="G11" s="17" t="s">
         <v>5</v>
       </c>
       <c r="H11" s="2">
         <v>3</v>
       </c>
       <c r="I11" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="J11" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="12" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B12" s="8"/>
+      <c r="B12" s="25"/>
       <c r="C12" s="1">
         <v>7</v>
       </c>
@@ -886,19 +881,19 @@
       <c r="E12" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="G12" s="5"/>
+      <c r="G12" s="17"/>
       <c r="H12" s="2">
         <v>7</v>
       </c>
       <c r="I12" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="J12" s="20" t="s">
-        <v>33</v>
+        <v>31</v>
+      </c>
+      <c r="J12" s="13" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="13" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B13" s="9"/>
+      <c r="B13" s="26"/>
       <c r="C13" s="1">
         <v>10</v>
       </c>
@@ -908,19 +903,19 @@
       <c r="E13" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="G13" s="5"/>
+      <c r="G13" s="17"/>
       <c r="H13" s="2">
         <v>10</v>
       </c>
-      <c r="I13" s="20" t="s">
-        <v>34</v>
-      </c>
-      <c r="J13" s="4" t="s">
-        <v>35</v>
+      <c r="I13" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="J13" s="5" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="14" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B14" s="5" t="s">
+      <c r="B14" s="17" t="s">
         <v>6</v>
       </c>
       <c r="C14" s="1">
@@ -932,21 +927,21 @@
       <c r="E14" s="1">
         <v>292</v>
       </c>
-      <c r="G14" s="5" t="s">
+      <c r="G14" s="17" t="s">
         <v>6</v>
       </c>
       <c r="H14" s="2">
         <v>7</v>
       </c>
       <c r="I14" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="J14" s="4" t="s">
-        <v>36</v>
+        <v>33</v>
+      </c>
+      <c r="J14" s="5" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="15" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B15" s="5"/>
+      <c r="B15" s="17"/>
       <c r="C15" s="1">
         <v>14</v>
       </c>
@@ -956,19 +951,19 @@
       <c r="E15" s="1">
         <v>581</v>
       </c>
-      <c r="G15" s="5"/>
+      <c r="G15" s="17"/>
       <c r="H15" s="2">
         <v>14</v>
       </c>
       <c r="I15" s="4" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="J15" s="4" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="16" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B16" s="5"/>
+      <c r="B16" s="17"/>
       <c r="C16" s="4">
         <v>21</v>
       </c>
@@ -978,19 +973,19 @@
       <c r="E16" s="4">
         <v>1068</v>
       </c>
-      <c r="G16" s="5"/>
+      <c r="G16" s="17"/>
       <c r="H16" s="4">
         <v>21</v>
       </c>
-      <c r="I16" s="20" t="s">
-        <v>38</v>
-      </c>
-      <c r="J16" s="4" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="17" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B17" s="5" t="s">
+      <c r="I16" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="J16" s="5" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="17" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B17" s="17" t="s">
         <v>7</v>
       </c>
       <c r="C17" s="4">
@@ -1002,21 +997,21 @@
       <c r="E17" s="4">
         <v>352</v>
       </c>
-      <c r="G17" s="5" t="s">
+      <c r="G17" s="17" t="s">
         <v>7</v>
       </c>
       <c r="H17" s="4">
         <v>7</v>
       </c>
       <c r="I17" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="J17" s="4" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="18" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B18" s="5"/>
+        <v>36</v>
+      </c>
+      <c r="J17" s="5" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="18" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B18" s="17"/>
       <c r="C18" s="4">
         <v>14</v>
       </c>
@@ -1026,19 +1021,19 @@
       <c r="E18" s="4">
         <v>818</v>
       </c>
-      <c r="G18" s="5"/>
+      <c r="G18" s="17"/>
       <c r="H18" s="4">
         <v>14</v>
       </c>
-      <c r="I18" s="20" t="s">
-        <v>41</v>
-      </c>
-      <c r="J18" s="4" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="19" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B19" s="5"/>
+      <c r="I18" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="J18" s="5" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="19" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B19" s="17"/>
       <c r="C19" s="4">
         <v>21</v>
       </c>
@@ -1048,19 +1043,19 @@
       <c r="E19" s="4">
         <v>1174</v>
       </c>
-      <c r="G19" s="5"/>
+      <c r="G19" s="17"/>
       <c r="H19" s="4">
         <v>21</v>
       </c>
       <c r="I19" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="J19" s="20" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="20" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B20" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="J19" s="15" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="20" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B20" s="17" t="s">
         <v>8</v>
       </c>
       <c r="C20" s="4">
@@ -1072,13 +1067,13 @@
       <c r="E20" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="G20" s="17"/>
-      <c r="H20" s="16"/>
-      <c r="I20" s="14"/>
-      <c r="J20" s="13"/>
-    </row>
-    <row r="21" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B21" s="5"/>
+      <c r="G20" s="11"/>
+      <c r="H20" s="10"/>
+      <c r="I20" s="9"/>
+      <c r="J20" s="8"/>
+    </row>
+    <row r="21" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B21" s="17"/>
       <c r="C21" s="4">
         <v>75</v>
       </c>
@@ -1088,15 +1083,15 @@
       <c r="E21" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="G21" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="H21" s="5"/>
-      <c r="I21" s="5"/>
-      <c r="J21" s="5"/>
-    </row>
-    <row r="22" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B22" s="5"/>
+      <c r="G21" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="H21" s="17"/>
+      <c r="I21" s="17"/>
+      <c r="J21" s="17"/>
+    </row>
+    <row r="22" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B22" s="17"/>
       <c r="C22" s="4">
         <v>112</v>
       </c>
@@ -1106,17 +1101,17 @@
       <c r="E22" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="G22" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="H22" s="5"/>
-      <c r="I22" s="22" t="s">
-        <v>53</v>
-      </c>
-      <c r="J22" s="22"/>
-    </row>
-    <row r="23" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B23" s="5" t="s">
+      <c r="G22" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="H22" s="17"/>
+      <c r="I22" s="19" t="s">
+        <v>44</v>
+      </c>
+      <c r="J22" s="19"/>
+    </row>
+    <row r="23" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B23" s="17" t="s">
         <v>9</v>
       </c>
       <c r="C23" s="4">
@@ -1128,17 +1123,17 @@
       <c r="E23" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="G23" s="23" t="s">
+      <c r="G23" s="20" t="s">
+        <v>45</v>
+      </c>
+      <c r="H23" s="20"/>
+      <c r="I23" s="21" t="s">
         <v>54</v>
       </c>
-      <c r="H23" s="23"/>
-      <c r="I23" s="11" t="s">
-        <v>55</v>
-      </c>
-      <c r="J23" s="11"/>
-    </row>
-    <row r="24" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B24" s="5"/>
+      <c r="J23" s="21"/>
+    </row>
+    <row r="24" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B24" s="17"/>
       <c r="C24" s="4">
         <v>140</v>
       </c>
@@ -1148,17 +1143,17 @@
       <c r="E24" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="G24" s="24" t="s">
-        <v>56</v>
-      </c>
-      <c r="H24" s="24"/>
-      <c r="I24" s="25" t="s">
-        <v>57</v>
-      </c>
-      <c r="J24" s="25"/>
-    </row>
-    <row r="25" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B25" s="5"/>
+      <c r="G24" s="22" t="s">
+        <v>46</v>
+      </c>
+      <c r="H24" s="22"/>
+      <c r="I24" s="23" t="s">
+        <v>47</v>
+      </c>
+      <c r="J24" s="23"/>
+    </row>
+    <row r="25" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B25" s="17"/>
       <c r="C25" s="4">
         <v>210</v>
       </c>
@@ -1168,85 +1163,97 @@
       <c r="E25" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="G25" s="24"/>
-      <c r="H25" s="24"/>
-      <c r="I25" s="25"/>
-      <c r="J25" s="25"/>
-    </row>
-    <row r="27" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="G27" s="10"/>
-      <c r="H27" s="10"/>
-      <c r="I27" s="6" t="s">
+      <c r="G25" s="22"/>
+      <c r="H25" s="22"/>
+      <c r="I25" s="23"/>
+      <c r="J25" s="23"/>
+    </row>
+    <row r="27" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="G27" s="6"/>
+      <c r="H27" s="6"/>
+      <c r="I27" s="16" t="s">
+        <v>51</v>
+      </c>
+      <c r="J27" s="16"/>
+    </row>
+    <row r="28" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="G28" s="2" t="s">
         <v>27</v>
-      </c>
-      <c r="J27" s="6"/>
-    </row>
-    <row r="28" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="G28" s="2" t="s">
-        <v>28</v>
       </c>
       <c r="H28" s="2" t="s">
         <v>4</v>
       </c>
       <c r="I28" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="J28" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="J28" s="2" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="29" spans="2:10" ht="45" x14ac:dyDescent="0.25">
-      <c r="G29" s="5" t="s">
+      <c r="L28" s="27"/>
+    </row>
+    <row r="29" spans="2:12" ht="45" x14ac:dyDescent="0.25">
+      <c r="G29" s="17" t="s">
         <v>8</v>
       </c>
       <c r="H29" s="4">
         <v>37</v>
       </c>
-      <c r="I29" s="21" t="s">
-        <v>45</v>
-      </c>
-      <c r="J29" s="18" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="30" spans="2:10" ht="75" x14ac:dyDescent="0.25">
-      <c r="G30" s="5"/>
+      <c r="I29" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="J29" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="K29" s="27"/>
+    </row>
+    <row r="30" spans="2:12" ht="75" x14ac:dyDescent="0.25">
+      <c r="G30" s="17"/>
       <c r="H30" s="4">
         <v>75</v>
       </c>
-      <c r="I30" s="21" t="s">
-        <v>47</v>
-      </c>
-      <c r="J30" s="18" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="31" spans="2:10" ht="105" x14ac:dyDescent="0.25">
-      <c r="G31" s="5"/>
+      <c r="I30" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="J30" s="12" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="31" spans="2:12" ht="105" x14ac:dyDescent="0.25">
+      <c r="G31" s="17"/>
       <c r="H31" s="4">
         <v>112</v>
       </c>
-      <c r="I31" s="21" t="s">
-        <v>49</v>
-      </c>
-      <c r="J31" s="19" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="32" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="G32" s="15"/>
-      <c r="H32" s="16"/>
+      <c r="I31" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="J31" s="28" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="32" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="G32" s="18"/>
+      <c r="H32" s="10"/>
     </row>
     <row r="33" spans="7:8" x14ac:dyDescent="0.25">
-      <c r="G33" s="15"/>
-      <c r="H33" s="16"/>
+      <c r="G33" s="18"/>
+      <c r="H33" s="10"/>
     </row>
     <row r="34" spans="7:8" x14ac:dyDescent="0.25">
-      <c r="G34" s="15"/>
-      <c r="H34" s="16"/>
+      <c r="G34" s="18"/>
+      <c r="H34" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="G11:G13"/>
+    <mergeCell ref="G14:G16"/>
+    <mergeCell ref="G17:G19"/>
+    <mergeCell ref="I9:J9"/>
+    <mergeCell ref="B23:B25"/>
+    <mergeCell ref="D9:E9"/>
+    <mergeCell ref="B11:B13"/>
+    <mergeCell ref="B14:B16"/>
+    <mergeCell ref="B17:B19"/>
+    <mergeCell ref="B20:B22"/>
     <mergeCell ref="I27:J27"/>
     <mergeCell ref="G29:G31"/>
     <mergeCell ref="G32:G34"/>
@@ -1257,16 +1264,6 @@
     <mergeCell ref="I23:J23"/>
     <mergeCell ref="G24:H25"/>
     <mergeCell ref="I24:J25"/>
-    <mergeCell ref="G11:G13"/>
-    <mergeCell ref="G14:G16"/>
-    <mergeCell ref="G17:G19"/>
-    <mergeCell ref="I9:J9"/>
-    <mergeCell ref="B23:B25"/>
-    <mergeCell ref="D9:E9"/>
-    <mergeCell ref="B11:B13"/>
-    <mergeCell ref="B14:B16"/>
-    <mergeCell ref="B17:B19"/>
-    <mergeCell ref="B20:B22"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Adição de algumas comparações com o modelo
</commit_message>
<xml_diff>
--- a/Comparaçoes/ComparaçãoEntreHeurísticas.xlsx
+++ b/Comparaçoes/ComparaçãoEntreHeurísticas.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="67">
   <si>
     <t>Problemas</t>
   </si>
@@ -286,6 +286,33 @@
       </rPr>
       <t>,87,34,30,84,7,8,89,96,63,48,73,76,35,93,124,126,52,33,105,111,16,59,79,121,15,78,133,88,94,122,77,14,80,10,113,3,62,149,125,22,21,150,115,44,71,45,4,128,104,68,119,91,106,13,92,54,46,138,134,90,56,83,26,146,75,141,25,20,51,109,43,81,110,58,55,86,29,135,50,70,108,67,47,120,42,37,2,9,28,6,139,40,53,118,24,12,19,99,114,102,32,131,38,23,127,69,36,61,64</t>
     </r>
+  </si>
+  <si>
+    <t>Modelo</t>
+  </si>
+  <si>
+    <t>1,24,13,16,27,8,28,6,12,9,5,21,2,20,10,4,15,18,14,22,17</t>
+  </si>
+  <si>
+    <t>1,9,11,</t>
+  </si>
+  <si>
+    <t>1,8,11,9,13,7,6</t>
+  </si>
+  <si>
+    <t>1,8,11,9,13,7,6,12,4,3</t>
+  </si>
+  <si>
+    <t>1,21,2,20,10,4,15</t>
+  </si>
+  <si>
+    <t>1,28,6,5,21,2,20,10,4,15,18,14,22,17</t>
+  </si>
+  <si>
+    <t>1,28,12,6,9,5,21,2,20,10,13,24,27,16,19,15,4,18,14,22,17</t>
+  </si>
+  <si>
+    <t>1,103,77,52,133,122,131,67,20,25,26,83,141,55,99,19,2,29,120,51,49,144,71,119,145,123,106,13,74,44,64,72,112,59,15,79,78,</t>
   </si>
 </sst>
 </file>
@@ -400,7 +427,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -441,44 +468,53 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -783,8 +819,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B9:O34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F17" workbookViewId="0">
-      <selection activeCell="K29" sqref="K29"/>
+    <sheetView tabSelected="1" topLeftCell="F20" workbookViewId="0">
+      <selection activeCell="K30" sqref="K30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -796,22 +832,23 @@
     <col min="7" max="7" width="10.85546875" customWidth="1"/>
     <col min="8" max="8" width="17.85546875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="48.28515625" customWidth="1"/>
-    <col min="10" max="10" width="48.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="48.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="9" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B9" s="3"/>
       <c r="C9" s="1"/>
-      <c r="D9" s="16" t="s">
+      <c r="D9" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="E9" s="16"/>
+      <c r="E9" s="20"/>
       <c r="G9" s="6"/>
       <c r="H9" s="6"/>
-      <c r="I9" s="16" t="s">
+      <c r="I9" s="20" t="s">
         <v>51</v>
       </c>
-      <c r="J9" s="16"/>
+      <c r="J9" s="20"/>
+      <c r="K9" s="20"/>
     </row>
     <row r="10" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B10" s="3" t="s">
@@ -838,14 +875,16 @@
       <c r="J10" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="K10" s="7"/>
+      <c r="K10" s="19" t="s">
+        <v>58</v>
+      </c>
       <c r="L10" s="7"/>
       <c r="M10" s="7"/>
       <c r="N10" s="7"/>
       <c r="O10" s="7"/>
     </row>
     <row r="11" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B11" s="24" t="s">
+      <c r="B11" s="28" t="s">
         <v>5</v>
       </c>
       <c r="C11" s="1">
@@ -857,7 +896,7 @@
       <c r="E11" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="G11" s="17" t="s">
+      <c r="G11" s="21" t="s">
         <v>5</v>
       </c>
       <c r="H11" s="2">
@@ -869,9 +908,12 @@
       <c r="J11" s="4" t="s">
         <v>30</v>
       </c>
+      <c r="K11" s="18" t="s">
+        <v>60</v>
+      </c>
     </row>
     <row r="12" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B12" s="25"/>
+      <c r="B12" s="29"/>
       <c r="C12" s="1">
         <v>7</v>
       </c>
@@ -881,7 +923,7 @@
       <c r="E12" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="G12" s="17"/>
+      <c r="G12" s="21"/>
       <c r="H12" s="2">
         <v>7</v>
       </c>
@@ -891,9 +933,12 @@
       <c r="J12" s="13" t="s">
         <v>48</v>
       </c>
+      <c r="K12" s="18" t="s">
+        <v>61</v>
+      </c>
     </row>
     <row r="13" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B13" s="26"/>
+      <c r="B13" s="30"/>
       <c r="C13" s="1">
         <v>10</v>
       </c>
@@ -903,7 +948,7 @@
       <c r="E13" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="G13" s="17"/>
+      <c r="G13" s="21"/>
       <c r="H13" s="2">
         <v>10</v>
       </c>
@@ -913,9 +958,12 @@
       <c r="J13" s="5" t="s">
         <v>49</v>
       </c>
+      <c r="K13" s="18" t="s">
+        <v>62</v>
+      </c>
     </row>
     <row r="14" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B14" s="17" t="s">
+      <c r="B14" s="21" t="s">
         <v>6</v>
       </c>
       <c r="C14" s="1">
@@ -927,7 +975,7 @@
       <c r="E14" s="1">
         <v>292</v>
       </c>
-      <c r="G14" s="17" t="s">
+      <c r="G14" s="21" t="s">
         <v>6</v>
       </c>
       <c r="H14" s="2">
@@ -939,9 +987,12 @@
       <c r="J14" s="5" t="s">
         <v>33</v>
       </c>
+      <c r="K14" s="18" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="15" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B15" s="17"/>
+      <c r="B15" s="21"/>
       <c r="C15" s="1">
         <v>14</v>
       </c>
@@ -951,7 +1002,7 @@
       <c r="E15" s="1">
         <v>581</v>
       </c>
-      <c r="G15" s="17"/>
+      <c r="G15" s="21"/>
       <c r="H15" s="2">
         <v>14</v>
       </c>
@@ -961,9 +1012,12 @@
       <c r="J15" s="4" t="s">
         <v>34</v>
       </c>
+      <c r="K15" s="18" t="s">
+        <v>59</v>
+      </c>
     </row>
     <row r="16" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B16" s="17"/>
+      <c r="B16" s="21"/>
       <c r="C16" s="4">
         <v>21</v>
       </c>
@@ -973,7 +1027,7 @@
       <c r="E16" s="4">
         <v>1068</v>
       </c>
-      <c r="G16" s="17"/>
+      <c r="G16" s="21"/>
       <c r="H16" s="4">
         <v>21</v>
       </c>
@@ -983,9 +1037,12 @@
       <c r="J16" s="5" t="s">
         <v>50</v>
       </c>
+      <c r="K16" s="18" t="s">
+        <v>59</v>
+      </c>
     </row>
     <row r="17" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B17" s="17" t="s">
+      <c r="B17" s="21" t="s">
         <v>7</v>
       </c>
       <c r="C17" s="4">
@@ -997,7 +1054,7 @@
       <c r="E17" s="4">
         <v>352</v>
       </c>
-      <c r="G17" s="17" t="s">
+      <c r="G17" s="21" t="s">
         <v>7</v>
       </c>
       <c r="H17" s="4">
@@ -1009,9 +1066,12 @@
       <c r="J17" s="5" t="s">
         <v>36</v>
       </c>
+      <c r="K17" s="18" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="18" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B18" s="17"/>
+      <c r="B18" s="21"/>
       <c r="C18" s="4">
         <v>14</v>
       </c>
@@ -1021,7 +1081,7 @@
       <c r="E18" s="4">
         <v>818</v>
       </c>
-      <c r="G18" s="17"/>
+      <c r="G18" s="21"/>
       <c r="H18" s="4">
         <v>14</v>
       </c>
@@ -1031,9 +1091,12 @@
       <c r="J18" s="5" t="s">
         <v>52</v>
       </c>
+      <c r="K18" s="18" t="s">
+        <v>64</v>
+      </c>
     </row>
     <row r="19" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B19" s="17"/>
+      <c r="B19" s="21"/>
       <c r="C19" s="4">
         <v>21</v>
       </c>
@@ -1043,7 +1106,7 @@
       <c r="E19" s="4">
         <v>1174</v>
       </c>
-      <c r="G19" s="17"/>
+      <c r="G19" s="21"/>
       <c r="H19" s="4">
         <v>21</v>
       </c>
@@ -1053,9 +1116,12 @@
       <c r="J19" s="15" t="s">
         <v>53</v>
       </c>
+      <c r="K19" s="18" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="20" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B20" s="17" t="s">
+      <c r="B20" s="21" t="s">
         <v>8</v>
       </c>
       <c r="C20" s="4">
@@ -1073,7 +1139,7 @@
       <c r="J20" s="8"/>
     </row>
     <row r="21" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B21" s="17"/>
+      <c r="B21" s="21"/>
       <c r="C21" s="4">
         <v>75</v>
       </c>
@@ -1083,15 +1149,15 @@
       <c r="E21" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="G21" s="17" t="s">
+      <c r="G21" s="21" t="s">
         <v>42</v>
       </c>
-      <c r="H21" s="17"/>
-      <c r="I21" s="17"/>
-      <c r="J21" s="17"/>
+      <c r="H21" s="21"/>
+      <c r="I21" s="21"/>
+      <c r="J21" s="21"/>
     </row>
     <row r="22" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B22" s="17"/>
+      <c r="B22" s="21"/>
       <c r="C22" s="4">
         <v>112</v>
       </c>
@@ -1101,17 +1167,18 @@
       <c r="E22" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="G22" s="17" t="s">
+      <c r="G22" s="21" t="s">
         <v>43</v>
       </c>
-      <c r="H22" s="17"/>
-      <c r="I22" s="19" t="s">
+      <c r="H22" s="21"/>
+      <c r="I22" s="23" t="s">
         <v>44</v>
       </c>
-      <c r="J22" s="19"/>
+      <c r="J22" s="23"/>
+      <c r="K22" s="16"/>
     </row>
     <row r="23" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B23" s="17" t="s">
+      <c r="B23" s="21" t="s">
         <v>9</v>
       </c>
       <c r="C23" s="4">
@@ -1123,17 +1190,17 @@
       <c r="E23" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="G23" s="20" t="s">
+      <c r="G23" s="24" t="s">
         <v>45</v>
       </c>
-      <c r="H23" s="20"/>
-      <c r="I23" s="21" t="s">
+      <c r="H23" s="24"/>
+      <c r="I23" s="25" t="s">
         <v>54</v>
       </c>
-      <c r="J23" s="21"/>
+      <c r="J23" s="25"/>
     </row>
     <row r="24" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B24" s="17"/>
+      <c r="B24" s="21"/>
       <c r="C24" s="4">
         <v>140</v>
       </c>
@@ -1143,17 +1210,17 @@
       <c r="E24" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="G24" s="22" t="s">
+      <c r="G24" s="26" t="s">
         <v>46</v>
       </c>
-      <c r="H24" s="22"/>
-      <c r="I24" s="23" t="s">
+      <c r="H24" s="26"/>
+      <c r="I24" s="27" t="s">
         <v>47</v>
       </c>
-      <c r="J24" s="23"/>
+      <c r="J24" s="27"/>
     </row>
     <row r="25" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B25" s="17"/>
+      <c r="B25" s="21"/>
       <c r="C25" s="4">
         <v>210</v>
       </c>
@@ -1163,18 +1230,19 @@
       <c r="E25" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="G25" s="22"/>
-      <c r="H25" s="22"/>
-      <c r="I25" s="23"/>
-      <c r="J25" s="23"/>
+      <c r="G25" s="26"/>
+      <c r="H25" s="26"/>
+      <c r="I25" s="27"/>
+      <c r="J25" s="27"/>
     </row>
     <row r="27" spans="2:12" x14ac:dyDescent="0.25">
       <c r="G27" s="6"/>
       <c r="H27" s="6"/>
-      <c r="I27" s="16" t="s">
+      <c r="I27" s="20" t="s">
         <v>51</v>
       </c>
-      <c r="J27" s="16"/>
+      <c r="J27" s="20"/>
+      <c r="K27" s="20"/>
     </row>
     <row r="28" spans="2:12" x14ac:dyDescent="0.25">
       <c r="G28" s="2" t="s">
@@ -1189,10 +1257,13 @@
       <c r="J28" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="L28" s="27"/>
+      <c r="K28" s="18" t="s">
+        <v>58</v>
+      </c>
+      <c r="L28" s="16"/>
     </row>
     <row r="29" spans="2:12" ht="45" x14ac:dyDescent="0.25">
-      <c r="G29" s="17" t="s">
+      <c r="G29" s="21" t="s">
         <v>8</v>
       </c>
       <c r="H29" s="4">
@@ -1204,10 +1275,12 @@
       <c r="J29" s="12" t="s">
         <v>55</v>
       </c>
-      <c r="K29" s="27"/>
+      <c r="K29" s="31" t="s">
+        <v>66</v>
+      </c>
     </row>
     <row r="30" spans="2:12" ht="75" x14ac:dyDescent="0.25">
-      <c r="G30" s="17"/>
+      <c r="G30" s="21"/>
       <c r="H30" s="4">
         <v>75</v>
       </c>
@@ -1217,29 +1290,31 @@
       <c r="J30" s="12" t="s">
         <v>56</v>
       </c>
+      <c r="K30" s="18"/>
     </row>
     <row r="31" spans="2:12" ht="105" x14ac:dyDescent="0.25">
-      <c r="G31" s="17"/>
+      <c r="G31" s="21"/>
       <c r="H31" s="4">
         <v>112</v>
       </c>
       <c r="I31" s="14" t="s">
         <v>41</v>
       </c>
-      <c r="J31" s="28" t="s">
+      <c r="J31" s="17" t="s">
         <v>57</v>
       </c>
+      <c r="K31" s="18"/>
     </row>
     <row r="32" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="G32" s="18"/>
+      <c r="G32" s="22"/>
       <c r="H32" s="10"/>
     </row>
     <row r="33" spans="7:8" x14ac:dyDescent="0.25">
-      <c r="G33" s="18"/>
+      <c r="G33" s="22"/>
       <c r="H33" s="10"/>
     </row>
     <row r="34" spans="7:8" x14ac:dyDescent="0.25">
-      <c r="G34" s="18"/>
+      <c r="G34" s="22"/>
       <c r="H34" s="10"/>
     </row>
   </sheetData>
@@ -1247,14 +1322,13 @@
     <mergeCell ref="G11:G13"/>
     <mergeCell ref="G14:G16"/>
     <mergeCell ref="G17:G19"/>
-    <mergeCell ref="I9:J9"/>
     <mergeCell ref="B23:B25"/>
     <mergeCell ref="D9:E9"/>
     <mergeCell ref="B11:B13"/>
     <mergeCell ref="B14:B16"/>
     <mergeCell ref="B17:B19"/>
     <mergeCell ref="B20:B22"/>
-    <mergeCell ref="I27:J27"/>
+    <mergeCell ref="I9:K9"/>
     <mergeCell ref="G29:G31"/>
     <mergeCell ref="G32:G34"/>
     <mergeCell ref="G21:J21"/>
@@ -1264,6 +1338,7 @@
     <mergeCell ref="I23:J23"/>
     <mergeCell ref="G24:H25"/>
     <mergeCell ref="I24:J25"/>
+    <mergeCell ref="I27:K27"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Adição de um novo tipo de cálculo de distância(Utilizado nos casos att48 e att532)
</commit_message>
<xml_diff>
--- a/Comparaçoes/ComparaçãoEntreHeurísticas.xlsx
+++ b/Comparaçoes/ComparaçãoEntreHeurísticas.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="68">
   <si>
     <t>Problemas</t>
   </si>
@@ -313,6 +313,9 @@
   </si>
   <si>
     <t>1,103,77,52,133,122,131,67,20,25,26,83,141,55,99,19,2,29,120,51,49,144,71,119,145,123,106,13,74,44,64,72,112,59,15,79,78,</t>
+  </si>
+  <si>
+    <t>1,73,88,78,91,149,71,122,127,141,114,25,110,33,38,20,29,70,137,102,108,56,72,124,125,49,136,13,15,63,98,46,138,14,45,16,126,80,134,75,93,54,5,95,48,143,76,77,96,135,85,97,133,129,61,66,118,39,32,53,41,117,109,131,128,101,139,69,43,12,74,119,104,4,44</t>
   </si>
 </sst>
 </file>
@@ -427,7 +430,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -480,10 +483,25 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
@@ -502,18 +520,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -819,8 +825,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B9:O34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F20" workbookViewId="0">
-      <selection activeCell="K30" sqref="K30"/>
+    <sheetView tabSelected="1" topLeftCell="F19" workbookViewId="0">
+      <selection activeCell="J29" sqref="J29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -838,17 +844,17 @@
     <row r="9" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B9" s="3"/>
       <c r="C9" s="1"/>
-      <c r="D9" s="20" t="s">
+      <c r="D9" s="23" t="s">
         <v>3</v>
       </c>
-      <c r="E9" s="20"/>
+      <c r="E9" s="23"/>
       <c r="G9" s="6"/>
       <c r="H9" s="6"/>
-      <c r="I9" s="20" t="s">
+      <c r="I9" s="23" t="s">
         <v>51</v>
       </c>
-      <c r="J9" s="20"/>
-      <c r="K9" s="20"/>
+      <c r="J9" s="23"/>
+      <c r="K9" s="23"/>
     </row>
     <row r="10" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B10" s="3" t="s">
@@ -884,7 +890,7 @@
       <c r="O10" s="7"/>
     </row>
     <row r="11" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B11" s="28" t="s">
+      <c r="B11" s="24" t="s">
         <v>5</v>
       </c>
       <c r="C11" s="1">
@@ -896,7 +902,7 @@
       <c r="E11" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="G11" s="21" t="s">
+      <c r="G11" s="22" t="s">
         <v>5</v>
       </c>
       <c r="H11" s="2">
@@ -913,7 +919,7 @@
       </c>
     </row>
     <row r="12" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B12" s="29"/>
+      <c r="B12" s="25"/>
       <c r="C12" s="1">
         <v>7</v>
       </c>
@@ -923,7 +929,7 @@
       <c r="E12" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="G12" s="21"/>
+      <c r="G12" s="22"/>
       <c r="H12" s="2">
         <v>7</v>
       </c>
@@ -938,7 +944,7 @@
       </c>
     </row>
     <row r="13" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B13" s="30"/>
+      <c r="B13" s="26"/>
       <c r="C13" s="1">
         <v>10</v>
       </c>
@@ -948,7 +954,7 @@
       <c r="E13" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="G13" s="21"/>
+      <c r="G13" s="22"/>
       <c r="H13" s="2">
         <v>10</v>
       </c>
@@ -963,7 +969,7 @@
       </c>
     </row>
     <row r="14" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B14" s="21" t="s">
+      <c r="B14" s="22" t="s">
         <v>6</v>
       </c>
       <c r="C14" s="1">
@@ -975,7 +981,7 @@
       <c r="E14" s="1">
         <v>292</v>
       </c>
-      <c r="G14" s="21" t="s">
+      <c r="G14" s="22" t="s">
         <v>6</v>
       </c>
       <c r="H14" s="2">
@@ -992,7 +998,7 @@
       </c>
     </row>
     <row r="15" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B15" s="21"/>
+      <c r="B15" s="22"/>
       <c r="C15" s="1">
         <v>14</v>
       </c>
@@ -1002,7 +1008,7 @@
       <c r="E15" s="1">
         <v>581</v>
       </c>
-      <c r="G15" s="21"/>
+      <c r="G15" s="22"/>
       <c r="H15" s="2">
         <v>14</v>
       </c>
@@ -1017,7 +1023,7 @@
       </c>
     </row>
     <row r="16" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B16" s="21"/>
+      <c r="B16" s="22"/>
       <c r="C16" s="4">
         <v>21</v>
       </c>
@@ -1027,7 +1033,7 @@
       <c r="E16" s="4">
         <v>1068</v>
       </c>
-      <c r="G16" s="21"/>
+      <c r="G16" s="22"/>
       <c r="H16" s="4">
         <v>21</v>
       </c>
@@ -1042,7 +1048,7 @@
       </c>
     </row>
     <row r="17" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B17" s="21" t="s">
+      <c r="B17" s="22" t="s">
         <v>7</v>
       </c>
       <c r="C17" s="4">
@@ -1054,7 +1060,7 @@
       <c r="E17" s="4">
         <v>352</v>
       </c>
-      <c r="G17" s="21" t="s">
+      <c r="G17" s="22" t="s">
         <v>7</v>
       </c>
       <c r="H17" s="4">
@@ -1071,7 +1077,7 @@
       </c>
     </row>
     <row r="18" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B18" s="21"/>
+      <c r="B18" s="22"/>
       <c r="C18" s="4">
         <v>14</v>
       </c>
@@ -1081,7 +1087,7 @@
       <c r="E18" s="4">
         <v>818</v>
       </c>
-      <c r="G18" s="21"/>
+      <c r="G18" s="22"/>
       <c r="H18" s="4">
         <v>14</v>
       </c>
@@ -1096,7 +1102,7 @@
       </c>
     </row>
     <row r="19" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B19" s="21"/>
+      <c r="B19" s="22"/>
       <c r="C19" s="4">
         <v>21</v>
       </c>
@@ -1106,7 +1112,7 @@
       <c r="E19" s="4">
         <v>1174</v>
       </c>
-      <c r="G19" s="21"/>
+      <c r="G19" s="22"/>
       <c r="H19" s="4">
         <v>21</v>
       </c>
@@ -1121,7 +1127,7 @@
       </c>
     </row>
     <row r="20" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B20" s="21" t="s">
+      <c r="B20" s="22" t="s">
         <v>8</v>
       </c>
       <c r="C20" s="4">
@@ -1139,7 +1145,7 @@
       <c r="J20" s="8"/>
     </row>
     <row r="21" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B21" s="21"/>
+      <c r="B21" s="22"/>
       <c r="C21" s="4">
         <v>75</v>
       </c>
@@ -1149,15 +1155,15 @@
       <c r="E21" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="G21" s="21" t="s">
+      <c r="G21" s="22" t="s">
         <v>42</v>
       </c>
-      <c r="H21" s="21"/>
-      <c r="I21" s="21"/>
-      <c r="J21" s="21"/>
+      <c r="H21" s="22"/>
+      <c r="I21" s="22"/>
+      <c r="J21" s="22"/>
     </row>
     <row r="22" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B22" s="21"/>
+      <c r="B22" s="22"/>
       <c r="C22" s="4">
         <v>112</v>
       </c>
@@ -1167,18 +1173,18 @@
       <c r="E22" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="G22" s="21" t="s">
+      <c r="G22" s="22" t="s">
         <v>43</v>
       </c>
-      <c r="H22" s="21"/>
-      <c r="I22" s="23" t="s">
+      <c r="H22" s="22"/>
+      <c r="I22" s="28" t="s">
         <v>44</v>
       </c>
-      <c r="J22" s="23"/>
+      <c r="J22" s="28"/>
       <c r="K22" s="16"/>
     </row>
     <row r="23" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B23" s="21" t="s">
+      <c r="B23" s="22" t="s">
         <v>9</v>
       </c>
       <c r="C23" s="4">
@@ -1190,17 +1196,17 @@
       <c r="E23" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="G23" s="24" t="s">
+      <c r="G23" s="29" t="s">
         <v>45</v>
       </c>
-      <c r="H23" s="24"/>
-      <c r="I23" s="25" t="s">
+      <c r="H23" s="29"/>
+      <c r="I23" s="30" t="s">
         <v>54</v>
       </c>
-      <c r="J23" s="25"/>
+      <c r="J23" s="30"/>
     </row>
     <row r="24" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B24" s="21"/>
+      <c r="B24" s="22"/>
       <c r="C24" s="4">
         <v>140</v>
       </c>
@@ -1210,17 +1216,17 @@
       <c r="E24" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="G24" s="26" t="s">
+      <c r="G24" s="31" t="s">
         <v>46</v>
       </c>
-      <c r="H24" s="26"/>
-      <c r="I24" s="27" t="s">
+      <c r="H24" s="31"/>
+      <c r="I24" s="32" t="s">
         <v>47</v>
       </c>
-      <c r="J24" s="27"/>
+      <c r="J24" s="32"/>
     </row>
     <row r="25" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B25" s="21"/>
+      <c r="B25" s="22"/>
       <c r="C25" s="4">
         <v>210</v>
       </c>
@@ -1230,19 +1236,19 @@
       <c r="E25" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="G25" s="26"/>
-      <c r="H25" s="26"/>
-      <c r="I25" s="27"/>
-      <c r="J25" s="27"/>
+      <c r="G25" s="31"/>
+      <c r="H25" s="31"/>
+      <c r="I25" s="32"/>
+      <c r="J25" s="32"/>
     </row>
     <row r="27" spans="2:12" x14ac:dyDescent="0.25">
       <c r="G27" s="6"/>
       <c r="H27" s="6"/>
-      <c r="I27" s="20" t="s">
+      <c r="I27" s="23" t="s">
         <v>51</v>
       </c>
-      <c r="J27" s="20"/>
-      <c r="K27" s="20"/>
+      <c r="J27" s="23"/>
+      <c r="K27" s="23"/>
     </row>
     <row r="28" spans="2:12" x14ac:dyDescent="0.25">
       <c r="G28" s="2" t="s">
@@ -1263,7 +1269,7 @@
       <c r="L28" s="16"/>
     </row>
     <row r="29" spans="2:12" ht="45" x14ac:dyDescent="0.25">
-      <c r="G29" s="21" t="s">
+      <c r="G29" s="22" t="s">
         <v>8</v>
       </c>
       <c r="H29" s="4">
@@ -1275,12 +1281,12 @@
       <c r="J29" s="12" t="s">
         <v>55</v>
       </c>
-      <c r="K29" s="31" t="s">
+      <c r="K29" s="21" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="30" spans="2:12" ht="75" x14ac:dyDescent="0.25">
-      <c r="G30" s="21"/>
+      <c r="G30" s="22"/>
       <c r="H30" s="4">
         <v>75</v>
       </c>
@@ -1290,10 +1296,12 @@
       <c r="J30" s="12" t="s">
         <v>56</v>
       </c>
-      <c r="K30" s="18"/>
+      <c r="K30" s="20" t="s">
+        <v>67</v>
+      </c>
     </row>
     <row r="31" spans="2:12" ht="105" x14ac:dyDescent="0.25">
-      <c r="G31" s="21"/>
+      <c r="G31" s="22"/>
       <c r="H31" s="4">
         <v>112</v>
       </c>
@@ -1306,28 +1314,19 @@
       <c r="K31" s="18"/>
     </row>
     <row r="32" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="G32" s="22"/>
+      <c r="G32" s="27"/>
       <c r="H32" s="10"/>
     </row>
     <row r="33" spans="7:8" x14ac:dyDescent="0.25">
-      <c r="G33" s="22"/>
+      <c r="G33" s="27"/>
       <c r="H33" s="10"/>
     </row>
     <row r="34" spans="7:8" x14ac:dyDescent="0.25">
-      <c r="G34" s="22"/>
+      <c r="G34" s="27"/>
       <c r="H34" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="G11:G13"/>
-    <mergeCell ref="G14:G16"/>
-    <mergeCell ref="G17:G19"/>
-    <mergeCell ref="B23:B25"/>
-    <mergeCell ref="D9:E9"/>
-    <mergeCell ref="B11:B13"/>
-    <mergeCell ref="B14:B16"/>
-    <mergeCell ref="B17:B19"/>
-    <mergeCell ref="B20:B22"/>
     <mergeCell ref="I9:K9"/>
     <mergeCell ref="G29:G31"/>
     <mergeCell ref="G32:G34"/>
@@ -1339,6 +1338,15 @@
     <mergeCell ref="G24:H25"/>
     <mergeCell ref="I24:J25"/>
     <mergeCell ref="I27:K27"/>
+    <mergeCell ref="G11:G13"/>
+    <mergeCell ref="G14:G16"/>
+    <mergeCell ref="G17:G19"/>
+    <mergeCell ref="B23:B25"/>
+    <mergeCell ref="D9:E9"/>
+    <mergeCell ref="B11:B13"/>
+    <mergeCell ref="B14:B16"/>
+    <mergeCell ref="B17:B19"/>
+    <mergeCell ref="B20:B22"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>